<commit_message>
Tims Arduino Pins aktualisiert
</commit_message>
<xml_diff>
--- a/Pins Arduino.xlsx
+++ b/Pins Arduino.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimBreuer\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BA6BB9-C728-455B-B824-A47CA5B5FF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDCD15D-5819-4437-B900-B6E0BA0D8423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9780" yWindow="1290" windowWidth="16290" windowHeight="11385" xr2:uid="{3D2ED62C-E83A-4130-96C2-79629FB24948}"/>
+    <workbookView xWindow="7140" yWindow="2160" windowWidth="21600" windowHeight="11385" xr2:uid="{3D2ED62C-E83A-4130-96C2-79629FB24948}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -94,22 +92,22 @@
     <t>Bluetooth4</t>
   </si>
   <si>
+    <t>Blue6SEL</t>
+  </si>
+  <si>
     <t>A10</t>
   </si>
   <si>
+    <t>Blue2CMD</t>
+  </si>
+  <si>
     <t>A9</t>
   </si>
   <si>
     <t>Blue1DAT</t>
   </si>
   <si>
-    <t>Blue2CMD</t>
-  </si>
-  <si>
     <t>Blue7CLK</t>
-  </si>
-  <si>
-    <t>Blue6SEL</t>
   </si>
 </sst>
 </file>
@@ -464,10 +462,10 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -554,7 +552,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -600,23 +598,23 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
         <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>22</v>
@@ -624,7 +622,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19">
         <v>12</v>

</xml_diff>